<commit_message>
Raghav Bansal Backup  07.11.2019 07.46 pm
</commit_message>
<xml_diff>
--- a/SocietyHead/UploadCertificationData.xlsx
+++ b/SocietyHead/UploadCertificationData.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCAS\SocietyHead\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6A2A94-4B8E-47E6-B42E-A42F7FB0FDE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B57111-DB36-46F4-B258-112BF32D45B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DRCKJBhPdGH9ntzMEvM0r0cFNcH9EVbCbTGEpR+EB2OHxe6aR8TWxxWJkqGRILb/fDzNDQ0sfXsfmb9xv6y5mg==" workbookSaltValue="0HUrxK8MrZPZMIPAaKNMhw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participation" sheetId="1" r:id="rId1"/>
@@ -399,9 +399,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,16 +423,12 @@
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="2">
-        <v>17103001</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="2">
-        <v>17103002</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1934,7 +1930,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2141,18 +2137,14 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="2">
-        <v>17103003</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="2">
-        <v>17103004</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2252,9 +2244,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2277,16 +2269,12 @@
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="2">
-        <v>17103005</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="2">
-        <v>17103006</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Raghav Bansal Changes 09.11.2019 04.28pm
</commit_message>
<xml_diff>
--- a/SocietyHead/UploadCertificationData.xlsx
+++ b/SocietyHead/UploadCertificationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCAS\SocietyHead\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B57111-DB36-46F4-B258-112BF32D45B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF99C7B6-99A3-46D2-AC3A-74D07E677071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DRCKJBhPdGH9ntzMEvM0r0cFNcH9EVbCbTGEpR+EB2OHxe6aR8TWxxWJkqGRILb/fDzNDQ0sfXsfmb9xv6y5mg==" workbookSaltValue="0HUrxK8MrZPZMIPAaKNMhw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>Sno</t>
   </si>
@@ -39,13 +39,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Team_name</t>
-  </si>
-  <si>
     <t>Position</t>
-  </si>
-  <si>
-    <t>Task_Organized</t>
   </si>
 </sst>
 </file>
@@ -83,7 +77,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,16 +100,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +413,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B3"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,7 +1929,7 @@
       <c r="C300" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="67XQOHxXCGoksTVQxPH32cv5f7s23lXs+DwrP7fmk8+rGRYTeqrmulN40gy1VYwPD1LY4eyI3X7isq9jRiYqkQ==" saltValue="z4+KaDxrGiPGp0E+W1rYBg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WQkmxWyLASJ90a8GDyZOA2enCTJKyWiDDiIDE7wQhh/XAZPSvbG5k1yAHPS2lFR9WBkZ0IkK6s/CtAGmz+2Vfw==" saltValue="6PV3fBDTgbq2CkXh4AqdZw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1929,16 +1941,17 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27:B29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1951,291 +1964,249 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>11</v>
-      </c>
+      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="BA50kxlqUxWlZBMqJAhug12KtHW6O71meMlWmWuZcN9zCkfjEGUq7FZVUS4Vh4W9oHLhxfpuPmiPiPcQfuqC6A==" saltValue="sCAzP4RazUDVgmHz6rHbOQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nvaVbLBlkCVlJix4lYXpElqj50gTt8/fEM0+oVCEKKgBMV5ihbH9LWV7Acer1oDos4F/3XxZ7kzkg7GZhdnpwQ==" saltValue="i+p/EJkxUfGZTY8dflUMbg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2246,224 +2217,183 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.44140625" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1jiyroYdaAUgAWjRNjZrW7JtOa5YhgQfBqnb1PNaB8EYzey6KRdUhjfWynpqIyeFqWrYsDR8ZaZcywB/0AG2Nw==" saltValue="/+CRyPwLv9iuUUt1eJIgmg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2svtNh4oXDgNm3+TC/oTHHKywprc27rxILUjnK6r/w4e+Tl5tm49UsNZq6niPvgaigitYyMOkRTY5a2A9Xe22g==" saltValue="+hJrUt609hGJdRCiCVyl6g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>